<commit_message>
added function to get list and default values
</commit_message>
<xml_diff>
--- a/conditions_output.xlsx
+++ b/conditions_output.xlsx
@@ -2738,10 +2738,10 @@
       <c r="H38" t="b">
         <v>1</v>
       </c>
-      <c r="I38" t="n">
-        <v>1</v>
-      </c>
-      <c r="J38" t="n">
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
         <v>1</v>
       </c>
       <c r="K38" t="n">
@@ -2775,14 +2775,14 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>QAimpression038display</t>
+          <t>QAimpression038video</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -2860,10 +2860,10 @@
       <c r="H40" t="b">
         <v>1</v>
       </c>
-      <c r="I40" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" t="n">
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
         <v>0</v>
       </c>
       <c r="K40" t="n">
@@ -2921,10 +2921,10 @@
       <c r="H41" t="b">
         <v>1</v>
       </c>
-      <c r="I41" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" t="n">
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
         <v>1</v>
       </c>
       <c r="K41" t="n">
@@ -2982,10 +2982,10 @@
       <c r="H42" t="b">
         <v>1</v>
       </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" t="n">
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
         <v>1</v>
       </c>
       <c r="K42" t="n">
@@ -3043,10 +3043,10 @@
       <c r="H43" t="b">
         <v>1</v>
       </c>
-      <c r="I43" t="n">
-        <v>1</v>
-      </c>
-      <c r="J43" t="n">
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" t="b">
         <v>1</v>
       </c>
       <c r="K43" t="n">
@@ -3385,14 +3385,14 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>QAimpression048display</t>
+          <t>QAimpression048video</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>1</v>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
@@ -3446,14 +3446,14 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>QAimpression049display</t>
+          <t>QAimpression049video</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -3507,14 +3507,14 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>QAimpression050display</t>
+          <t>QAimpression050video</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
@@ -3568,14 +3568,14 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>QAimpression051display</t>
+          <t>QAimpression051video</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -3629,14 +3629,14 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>QAimpression052display</t>
+          <t>QAimpression052video</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>1</v>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
@@ -3690,14 +3690,14 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>QAimpression053display</t>
+          <t>QAimpression053video</t>
         </is>
       </c>
       <c r="B54" t="n">
         <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -3751,14 +3751,14 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>QAimpression054display</t>
+          <t>QAimpression054video</t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>1</v>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
@@ -3812,14 +3812,14 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>QAimpression055display</t>
+          <t>QAimpression055video</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>1</v>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
@@ -4141,10 +4141,10 @@
       <c r="H61" t="b">
         <v>1</v>
       </c>
-      <c r="I61" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" t="n">
+      <c r="I61" t="b">
+        <v>1</v>
+      </c>
+      <c r="J61" t="b">
         <v>1</v>
       </c>
       <c r="K61" t="n">
@@ -4178,14 +4178,14 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>QAimpression061display</t>
+          <t>QAimpression061video</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
@@ -4263,10 +4263,10 @@
       <c r="H63" t="b">
         <v>1</v>
       </c>
-      <c r="I63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J63" t="n">
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+      <c r="J63" t="b">
         <v>0</v>
       </c>
       <c r="K63" t="n">
@@ -4324,10 +4324,10 @@
       <c r="H64" t="b">
         <v>1</v>
       </c>
-      <c r="I64" t="n">
-        <v>1</v>
-      </c>
-      <c r="J64" t="n">
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+      <c r="J64" t="b">
         <v>1</v>
       </c>
       <c r="K64" t="n">
@@ -4385,10 +4385,10 @@
       <c r="H65" t="b">
         <v>1</v>
       </c>
-      <c r="I65" t="n">
-        <v>0</v>
-      </c>
-      <c r="J65" t="n">
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+      <c r="J65" t="b">
         <v>1</v>
       </c>
       <c r="K65" t="n">
@@ -4446,10 +4446,10 @@
       <c r="H66" t="b">
         <v>1</v>
       </c>
-      <c r="I66" t="n">
-        <v>1</v>
-      </c>
-      <c r="J66" t="n">
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+      <c r="J66" t="b">
         <v>1</v>
       </c>
       <c r="K66" t="n">
@@ -4507,10 +4507,10 @@
       <c r="H67" t="b">
         <v>1</v>
       </c>
-      <c r="I67" t="n">
-        <v>0</v>
-      </c>
-      <c r="J67" t="n">
+      <c r="I67" t="b">
+        <v>0</v>
+      </c>
+      <c r="J67" t="b">
         <v>1</v>
       </c>
       <c r="K67" t="n">
@@ -4568,10 +4568,10 @@
       <c r="H68" t="b">
         <v>1</v>
       </c>
-      <c r="I68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J68" t="n">
+      <c r="I68" t="b">
+        <v>1</v>
+      </c>
+      <c r="J68" t="b">
         <v>1</v>
       </c>
       <c r="K68" t="n">
@@ -4629,10 +4629,10 @@
       <c r="H69" t="b">
         <v>1</v>
       </c>
-      <c r="I69" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" t="n">
+      <c r="I69" t="b">
+        <v>1</v>
+      </c>
+      <c r="J69" t="b">
         <v>1</v>
       </c>
       <c r="K69" t="n">
@@ -4666,14 +4666,14 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>QAimpression069display</t>
+          <t>QAimpression069video</t>
         </is>
       </c>
       <c r="B70" t="n">
         <v>1</v>
       </c>
       <c r="C70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D70" t="n">
         <v>0</v>
@@ -4751,10 +4751,10 @@
       <c r="H71" t="b">
         <v>1</v>
       </c>
-      <c r="I71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J71" t="n">
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71" t="b">
         <v>0</v>
       </c>
       <c r="K71" t="n">
@@ -4812,10 +4812,10 @@
       <c r="H72" t="b">
         <v>1</v>
       </c>
-      <c r="I72" t="n">
-        <v>1</v>
-      </c>
-      <c r="J72" t="n">
+      <c r="I72" t="b">
+        <v>1</v>
+      </c>
+      <c r="J72" t="b">
         <v>1</v>
       </c>
       <c r="K72" t="n">
@@ -4873,10 +4873,10 @@
       <c r="H73" t="b">
         <v>1</v>
       </c>
-      <c r="I73" t="n">
-        <v>0</v>
-      </c>
-      <c r="J73" t="n">
+      <c r="I73" t="b">
+        <v>0</v>
+      </c>
+      <c r="J73" t="b">
         <v>1</v>
       </c>
       <c r="K73" t="n">
@@ -4934,10 +4934,10 @@
       <c r="H74" t="b">
         <v>1</v>
       </c>
-      <c r="I74" t="n">
-        <v>1</v>
-      </c>
-      <c r="J74" t="n">
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" t="b">
         <v>1</v>
       </c>
       <c r="K74" t="n">
@@ -4995,10 +4995,10 @@
       <c r="H75" t="b">
         <v>1</v>
       </c>
-      <c r="I75" t="n">
-        <v>0</v>
-      </c>
-      <c r="J75" t="n">
+      <c r="I75" t="b">
+        <v>0</v>
+      </c>
+      <c r="J75" t="b">
         <v>1</v>
       </c>
       <c r="K75" t="n">
@@ -5056,10 +5056,10 @@
       <c r="H76" t="b">
         <v>1</v>
       </c>
-      <c r="I76" t="n">
-        <v>1</v>
-      </c>
-      <c r="J76" t="n">
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+      <c r="J76" t="b">
         <v>1</v>
       </c>
       <c r="K76" t="n">
@@ -5117,10 +5117,10 @@
       <c r="H77" t="b">
         <v>1</v>
       </c>
-      <c r="I77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J77" t="n">
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
+      <c r="J77" t="b">
         <v>1</v>
       </c>
       <c r="K77" t="n">
@@ -5178,10 +5178,10 @@
       <c r="H78" t="b">
         <v>1</v>
       </c>
-      <c r="I78" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" t="n">
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
+      <c r="J78" t="b">
         <v>1</v>
       </c>
       <c r="K78" t="n">
@@ -5239,10 +5239,10 @@
       <c r="H79" t="b">
         <v>1</v>
       </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="n">
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+      <c r="J79" t="b">
         <v>1</v>
       </c>
       <c r="K79" t="n">
@@ -5276,14 +5276,14 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>QAimpression079display</t>
+          <t>QAimpression079video</t>
         </is>
       </c>
       <c r="B80" t="n">
         <v>1</v>
       </c>
       <c r="C80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
@@ -5361,10 +5361,10 @@
       <c r="H81" t="b">
         <v>1</v>
       </c>
-      <c r="I81" t="n">
-        <v>0</v>
-      </c>
-      <c r="J81" t="n">
+      <c r="I81" t="b">
+        <v>0</v>
+      </c>
+      <c r="J81" t="b">
         <v>0</v>
       </c>
       <c r="K81" t="n">
@@ -5422,10 +5422,10 @@
       <c r="H82" t="b">
         <v>1</v>
       </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="n">
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82" t="b">
         <v>1</v>
       </c>
       <c r="K82" t="n">
@@ -5483,10 +5483,10 @@
       <c r="H83" t="b">
         <v>1</v>
       </c>
-      <c r="I83" t="n">
-        <v>0</v>
-      </c>
-      <c r="J83" t="n">
+      <c r="I83" t="b">
+        <v>0</v>
+      </c>
+      <c r="J83" t="b">
         <v>1</v>
       </c>
       <c r="K83" t="n">
@@ -5544,10 +5544,10 @@
       <c r="H84" t="b">
         <v>1</v>
       </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="n">
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="J84" t="b">
         <v>1</v>
       </c>
       <c r="K84" t="n">
@@ -5605,10 +5605,10 @@
       <c r="H85" t="b">
         <v>1</v>
       </c>
-      <c r="I85" t="n">
-        <v>0</v>
-      </c>
-      <c r="J85" t="n">
+      <c r="I85" t="b">
+        <v>0</v>
+      </c>
+      <c r="J85" t="b">
         <v>1</v>
       </c>
       <c r="K85" t="n">
@@ -5666,10 +5666,10 @@
       <c r="H86" t="b">
         <v>1</v>
       </c>
-      <c r="I86" t="n">
-        <v>1</v>
-      </c>
-      <c r="J86" t="n">
+      <c r="I86" t="b">
+        <v>1</v>
+      </c>
+      <c r="J86" t="b">
         <v>1</v>
       </c>
       <c r="K86" t="n">
@@ -5727,10 +5727,10 @@
       <c r="H87" t="b">
         <v>1</v>
       </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="n">
+      <c r="I87" t="b">
+        <v>1</v>
+      </c>
+      <c r="J87" t="b">
         <v>1</v>
       </c>
       <c r="K87" t="n">
@@ -5788,10 +5788,10 @@
       <c r="H88" t="b">
         <v>1</v>
       </c>
-      <c r="I88" t="n">
-        <v>0</v>
-      </c>
-      <c r="J88" t="n">
+      <c r="I88" t="b">
+        <v>0</v>
+      </c>
+      <c r="J88" t="b">
         <v>1</v>
       </c>
       <c r="K88" t="n">
@@ -5849,10 +5849,10 @@
       <c r="H89" t="b">
         <v>1</v>
       </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="n">
+      <c r="I89" t="b">
+        <v>1</v>
+      </c>
+      <c r="J89" t="b">
         <v>1</v>
       </c>
       <c r="K89" t="n">
@@ -5910,10 +5910,10 @@
       <c r="H90" t="b">
         <v>1</v>
       </c>
-      <c r="I90" t="n">
-        <v>1</v>
-      </c>
-      <c r="J90" t="n">
+      <c r="I90" t="b">
+        <v>1</v>
+      </c>
+      <c r="J90" t="b">
         <v>1</v>
       </c>
       <c r="K90" t="n">
@@ -5971,10 +5971,10 @@
       <c r="H91" t="b">
         <v>1</v>
       </c>
-      <c r="I91" t="n">
-        <v>1</v>
-      </c>
-      <c r="J91" t="n">
+      <c r="I91" t="b">
+        <v>1</v>
+      </c>
+      <c r="J91" t="b">
         <v>1</v>
       </c>
       <c r="K91" t="n">
@@ -6032,10 +6032,10 @@
       <c r="H92" t="b">
         <v>1</v>
       </c>
-      <c r="I92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J92" t="n">
+      <c r="I92" t="b">
+        <v>1</v>
+      </c>
+      <c r="J92" t="b">
         <v>1</v>
       </c>
       <c r="K92" t="n">
@@ -6093,10 +6093,10 @@
       <c r="H93" t="b">
         <v>1</v>
       </c>
-      <c r="I93" t="n">
-        <v>1</v>
-      </c>
-      <c r="J93" t="n">
+      <c r="I93" t="b">
+        <v>1</v>
+      </c>
+      <c r="J93" t="b">
         <v>1</v>
       </c>
       <c r="K93" t="n">
@@ -6154,10 +6154,10 @@
       <c r="H94" t="b">
         <v>1</v>
       </c>
-      <c r="I94" t="n">
-        <v>1</v>
-      </c>
-      <c r="J94" t="n">
+      <c r="I94" t="b">
+        <v>1</v>
+      </c>
+      <c r="J94" t="b">
         <v>1</v>
       </c>
       <c r="K94" t="n">
@@ -6215,10 +6215,10 @@
       <c r="H95" t="b">
         <v>1</v>
       </c>
-      <c r="I95" t="n">
-        <v>1</v>
-      </c>
-      <c r="J95" t="n">
+      <c r="I95" t="b">
+        <v>1</v>
+      </c>
+      <c r="J95" t="b">
         <v>1</v>
       </c>
       <c r="K95" t="n">
@@ -6276,10 +6276,10 @@
       <c r="H96" t="b">
         <v>1</v>
       </c>
-      <c r="I96" t="n">
-        <v>1</v>
-      </c>
-      <c r="J96" t="n">
+      <c r="I96" t="b">
+        <v>1</v>
+      </c>
+      <c r="J96" t="b">
         <v>1</v>
       </c>
       <c r="K96" t="n">
@@ -6886,10 +6886,10 @@
       <c r="H106" t="b">
         <v>1</v>
       </c>
-      <c r="I106" t="n">
-        <v>1</v>
-      </c>
-      <c r="J106" t="n">
+      <c r="I106" t="b">
+        <v>1</v>
+      </c>
+      <c r="J106" t="b">
         <v>1</v>
       </c>
       <c r="K106" t="n">
@@ -6923,14 +6923,14 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>QAimpression106display</t>
+          <t>QAimpression106video</t>
         </is>
       </c>
       <c r="B107" t="n">
         <v>1</v>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D107" t="n">
         <v>0</v>
@@ -7008,10 +7008,10 @@
       <c r="H108" t="b">
         <v>1</v>
       </c>
-      <c r="I108" t="n">
-        <v>0</v>
-      </c>
-      <c r="J108" t="n">
+      <c r="I108" t="b">
+        <v>0</v>
+      </c>
+      <c r="J108" t="b">
         <v>1</v>
       </c>
       <c r="K108" t="n">
@@ -7069,10 +7069,10 @@
       <c r="H109" t="b">
         <v>1</v>
       </c>
-      <c r="I109" t="n">
-        <v>0</v>
-      </c>
-      <c r="J109" t="n">
+      <c r="I109" t="b">
+        <v>0</v>
+      </c>
+      <c r="J109" t="b">
         <v>1</v>
       </c>
       <c r="K109" t="n">
@@ -7130,10 +7130,10 @@
       <c r="H110" t="b">
         <v>1</v>
       </c>
-      <c r="I110" t="n">
-        <v>1</v>
-      </c>
-      <c r="J110" t="n">
+      <c r="I110" t="b">
+        <v>1</v>
+      </c>
+      <c r="J110" t="b">
         <v>1</v>
       </c>
       <c r="K110" t="n">
@@ -7191,10 +7191,10 @@
       <c r="H111" t="b">
         <v>1</v>
       </c>
-      <c r="I111" t="n">
-        <v>1</v>
-      </c>
-      <c r="J111" t="n">
+      <c r="I111" t="b">
+        <v>1</v>
+      </c>
+      <c r="J111" t="b">
         <v>1</v>
       </c>
       <c r="K111" t="n">
@@ -8472,10 +8472,10 @@
       <c r="H132" t="b">
         <v>1</v>
       </c>
-      <c r="I132" t="n">
-        <v>1</v>
-      </c>
-      <c r="J132" t="n">
+      <c r="I132" t="b">
+        <v>1</v>
+      </c>
+      <c r="J132" t="b">
         <v>1</v>
       </c>
       <c r="K132" t="n">
@@ -8533,10 +8533,10 @@
       <c r="H133" t="b">
         <v>1</v>
       </c>
-      <c r="I133" t="n">
-        <v>1</v>
-      </c>
-      <c r="J133" t="n">
+      <c r="I133" t="b">
+        <v>1</v>
+      </c>
+      <c r="J133" t="b">
         <v>1</v>
       </c>
       <c r="K133" t="n">
@@ -8594,10 +8594,10 @@
       <c r="H134" t="b">
         <v>1</v>
       </c>
-      <c r="I134" t="n">
-        <v>0</v>
-      </c>
-      <c r="J134" t="n">
+      <c r="I134" t="b">
+        <v>0</v>
+      </c>
+      <c r="J134" t="b">
         <v>1</v>
       </c>
       <c r="K134" t="n">
@@ -8655,10 +8655,10 @@
       <c r="H135" t="b">
         <v>1</v>
       </c>
-      <c r="I135" t="n">
-        <v>0</v>
-      </c>
-      <c r="J135" t="n">
+      <c r="I135" t="b">
+        <v>0</v>
+      </c>
+      <c r="J135" t="b">
         <v>1</v>
       </c>
       <c r="K135" t="n">
@@ -8716,10 +8716,10 @@
       <c r="H136" t="b">
         <v>1</v>
       </c>
-      <c r="I136" t="n">
-        <v>0</v>
-      </c>
-      <c r="J136" t="n">
+      <c r="I136" t="b">
+        <v>0</v>
+      </c>
+      <c r="J136" t="b">
         <v>1</v>
       </c>
       <c r="K136" t="n">
@@ -8777,10 +8777,10 @@
       <c r="H137" t="b">
         <v>1</v>
       </c>
-      <c r="I137" t="n">
-        <v>0</v>
-      </c>
-      <c r="J137" t="n">
+      <c r="I137" t="b">
+        <v>0</v>
+      </c>
+      <c r="J137" t="b">
         <v>1</v>
       </c>
       <c r="K137" t="n">
@@ -8838,10 +8838,10 @@
       <c r="H138" t="b">
         <v>1</v>
       </c>
-      <c r="I138" t="n">
-        <v>1</v>
-      </c>
-      <c r="J138" t="n">
+      <c r="I138" t="b">
+        <v>1</v>
+      </c>
+      <c r="J138" t="b">
         <v>1</v>
       </c>
       <c r="K138" t="n">
@@ -8875,14 +8875,14 @@
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>QAimpression138display</t>
+          <t>QAimpression138video</t>
         </is>
       </c>
       <c r="B139" t="n">
         <v>1</v>
       </c>
       <c r="C139" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D139" t="n">
         <v>0</v>
@@ -8960,10 +8960,10 @@
       <c r="H140" t="b">
         <v>1</v>
       </c>
-      <c r="I140" t="n">
-        <v>1</v>
-      </c>
-      <c r="J140" t="n">
+      <c r="I140" t="b">
+        <v>1</v>
+      </c>
+      <c r="J140" t="b">
         <v>1</v>
       </c>
       <c r="K140" t="n">
@@ -8997,14 +8997,14 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>QAimpression140display</t>
+          <t>QAimpression140video</t>
         </is>
       </c>
       <c r="B141" t="n">
         <v>1</v>
       </c>
       <c r="C141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
@@ -9082,10 +9082,10 @@
       <c r="H142" t="b">
         <v>1</v>
       </c>
-      <c r="I142" t="n">
-        <v>1</v>
-      </c>
-      <c r="J142" t="n">
+      <c r="I142" t="b">
+        <v>1</v>
+      </c>
+      <c r="J142" t="b">
         <v>0</v>
       </c>
       <c r="K142" t="n">
@@ -9143,10 +9143,10 @@
       <c r="H143" t="b">
         <v>1</v>
       </c>
-      <c r="I143" t="n">
-        <v>1</v>
-      </c>
-      <c r="J143" t="n">
+      <c r="I143" t="b">
+        <v>1</v>
+      </c>
+      <c r="J143" t="b">
         <v>1</v>
       </c>
       <c r="K143" t="n">
@@ -9204,10 +9204,10 @@
       <c r="H144" t="b">
         <v>1</v>
       </c>
-      <c r="I144" t="n">
-        <v>1</v>
-      </c>
-      <c r="J144" t="n">
+      <c r="I144" t="b">
+        <v>1</v>
+      </c>
+      <c r="J144" t="b">
         <v>1</v>
       </c>
       <c r="K144" t="n">
@@ -9265,10 +9265,10 @@
       <c r="H145" t="b">
         <v>1</v>
       </c>
-      <c r="I145" t="n">
-        <v>1</v>
-      </c>
-      <c r="J145" t="n">
+      <c r="I145" t="b">
+        <v>1</v>
+      </c>
+      <c r="J145" t="b">
         <v>1</v>
       </c>
       <c r="K145" t="n">
@@ -9326,10 +9326,10 @@
       <c r="H146" t="b">
         <v>1</v>
       </c>
-      <c r="I146" t="n">
-        <v>0</v>
-      </c>
-      <c r="J146" t="n">
+      <c r="I146" t="b">
+        <v>0</v>
+      </c>
+      <c r="J146" t="b">
         <v>1</v>
       </c>
       <c r="K146" t="n">
@@ -9363,14 +9363,14 @@
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>QAimpression146display</t>
+          <t>QAimpression146video</t>
         </is>
       </c>
       <c r="B147" t="n">
         <v>1</v>
       </c>
       <c r="C147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D147" t="n">
         <v>0</v>

</xml_diff>